<commit_message>
Revert "Branche1 color added"
This reverts commit 5cd1d10f655ff04204e68b70c8a56211b2e1b8bb.
</commit_message>
<xml_diff>
--- a/Testing1.xlsx
+++ b/Testing1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas\Fichiers-Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D5F4AE7-2E33-4F58-8465-642FDE9B9300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A6F88F-2534-4096-8E0E-62DF8277DE61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4545AC7C-3C80-4303-8765-C5315DD7A457}"/>
   </bookViews>
@@ -55,18 +55,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -81,9 +75,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,7 +394,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -429,11 +422,9 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>